<commit_message>
Added some heatmaps to make model evaluation look a little better
Found a justified reason to add AO and no LS. Adjusted X13 to only find LS and AO only, no other regressors like weekday, Easter, etc.
</commit_message>
<xml_diff>
--- a/fcst_results/arima_with_outliers_summary_stats_IAH-Dom.xlsx
+++ b/fcst_results/arima_with_outliers_summary_stats_IAH-Dom.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,23 +468,23 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>AO2008Sep</t>
+          <t>AO2001Sep</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-371000</v>
+        <v>-443900</v>
       </c>
       <c r="C2" t="n">
-        <v>60800</v>
+        <v>98100</v>
       </c>
       <c r="D2" t="n">
-        <v>-6.103</v>
+        <v>-4.526</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-490000</v>
+        <v>-636000</v>
       </c>
       <c r="G2" t="n">
         <v>-252000</v>
@@ -493,226 +493,276 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>AO2020Mar</t>
+          <t>AO2008Sep</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>90680</v>
+        <v>-371000</v>
       </c>
       <c r="C3" t="n">
-        <v>30400</v>
+        <v>82100</v>
       </c>
       <c r="D3" t="n">
-        <v>2.984</v>
+        <v>-4.517</v>
       </c>
       <c r="E3" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>31100</v>
+        <v>-532000</v>
       </c>
       <c r="G3" t="n">
-        <v>150000</v>
+        <v>-210000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>ar.L1</t>
+          <t>AO2020Mar</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0687</v>
+        <v>90680</v>
       </c>
       <c r="C4" t="n">
-        <v>0.062</v>
+        <v>24400</v>
       </c>
       <c r="D4" t="n">
-        <v>1.109</v>
+        <v>3.716</v>
       </c>
       <c r="E4" t="n">
-        <v>0.267</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.053</v>
+        <v>42800</v>
       </c>
       <c r="G4" t="n">
-        <v>0.19</v>
+        <v>139000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>ar.L2</t>
+          <t>AO2021Jul</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8201000000000001</v>
+        <v>197600</v>
       </c>
       <c r="C5" t="n">
-        <v>0.052</v>
+        <v>644.773</v>
       </c>
       <c r="D5" t="n">
-        <v>15.807</v>
+        <v>306.456</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.718</v>
+        <v>196000</v>
       </c>
       <c r="G5" t="n">
-        <v>0.922</v>
+        <v>199000</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>ma.L1</t>
+          <t>ar.L1</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0034</v>
+        <v>-1.0988</v>
       </c>
       <c r="C6" t="n">
-        <v>0.103</v>
+        <v>0.102</v>
       </c>
       <c r="D6" t="n">
-        <v>0.034</v>
+        <v>-10.755</v>
       </c>
       <c r="E6" t="n">
-        <v>0.973</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.198</v>
+        <v>-1.299</v>
       </c>
       <c r="G6" t="n">
-        <v>0.205</v>
+        <v>-0.899</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>ma.L2</t>
+          <t>ar.L2</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.9965000000000001</v>
+        <v>-0.7786999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>0.073</v>
+        <v>0.108</v>
       </c>
       <c r="D7" t="n">
-        <v>-13.685</v>
+        <v>-7.19</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-1.139</v>
+        <v>-0.991</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.854</v>
+        <v>-0.5659999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>ar.S.L12</t>
+          <t>ma.L1</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9449</v>
+        <v>1.1724</v>
       </c>
       <c r="C8" t="n">
-        <v>0.046</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>20.528</v>
+        <v>13.826</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.855</v>
+        <v>1.006</v>
       </c>
       <c r="G8" t="n">
-        <v>1.035</v>
+        <v>1.339</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>ma.S.L12</t>
+          <t>ma.L2</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.9033</v>
+        <v>0.9308</v>
       </c>
       <c r="C9" t="n">
-        <v>0.081</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>-11.094</v>
+        <v>10.77</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.063</v>
+        <v>0.761</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.744</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>ma.S.L24</t>
+          <t>ar.S.L12</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.124</v>
+        <v>0.9405</v>
       </c>
       <c r="C10" t="n">
-        <v>0.053</v>
+        <v>0.04</v>
       </c>
       <c r="D10" t="n">
-        <v>2.349</v>
+        <v>23.283</v>
       </c>
       <c r="E10" t="n">
-        <v>0.019</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.021</v>
+        <v>0.861</v>
       </c>
       <c r="G10" t="n">
-        <v>0.228</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
+          <t>ma.S.L12</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.9023</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-12.43</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-1.045</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.76</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ma.S.L24</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1085</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.096</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
           <t>sigma2</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>14310000000</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="D11" t="n">
-        <v>451000000000</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>14300000000</v>
-      </c>
-      <c r="G11" t="n">
-        <v>14300000000</v>
+      <c r="B13" t="n">
+        <v>14210000000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1.814</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7830000000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>14200000000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>14200000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>